<commit_message>
[PURIO] Add script which handles whole flow
</commit_message>
<xml_diff>
--- a/category_check_list.xlsx
+++ b/category_check_list.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmakonst/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmakonst/Documents/Projects/food_facts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5831EC8-3D1C-874D-82E0-98E9A8447517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8479AD8-351D-0545-8464-B403704F0CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-58520" yWindow="-14740" windowWidth="33100" windowHeight="18680" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
+    <workbookView xWindow="-44080" yWindow="-16660" windowWidth="30220" windowHeight="17940" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>Category name</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Import Count</t>
   </si>
   <si>
-    <t>https://www.auchan.ro/bacanie/ceai-si-cafea/cafea-macinata/c?order=OrderByBestDiscountDESC</t>
-  </si>
-  <si>
     <t>Cafea macinata</t>
   </si>
   <si>
@@ -268,7 +265,143 @@
     <t>Non-Carbohydrated Juices</t>
   </si>
   <si>
-    <t>Import state</t>
+    <t>Supabase import</t>
+  </si>
+  <si>
+    <t>Imported</t>
+  </si>
+  <si>
+    <t>Import state (Local import)</t>
+  </si>
+  <si>
+    <t>SUM of imported</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Bere blonda Carlsberg, doza, 4 x 0.5 l
+Skipping duplicate product: Bere blonda Stella Artois 6 x 0.33 l
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Bere blonda Heineken, 0.33 l
+Skipping duplicate product: Bere blonda Zimbru, 0.5 l
+Skipping duplicate product: Bere blonda Heineken, 8 x 0.25 l
+Skipping duplicate product: Bere blonda San Miguel, 0.33 l
+Skipping duplicate product: Bere blonda Albacher, 0.5 l
+Skipping duplicate product: Bere blonda Grolsch, 6 x 0.5 l
+Skipping duplicate product: Bere blonda Ciuc, 6 x 0.5 l
+Skipping duplicate product: Bere blonda Lomza, 0.5 l
+Skipping duplicate product: Bere blonda Staropramen, 6 x 0.33 l
+Skipping duplicate product: Bere blonda Ciuc, 0.5 l
+Skipping duplicate product: Bere blonda Albacher, 0.33 l
+Skipped 5 records due to missing required fields or errors
+Skipped 13 records due to duplicate product names</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Import amount</t>
+  </si>
+  <si>
+    <t>Skipping duplicate product: Bautura racoritoare carbogazoasa OKF Aloe Vera Sparkling Original, 0.5 l
+Skipping duplicate product: Bautura carbogazoasa cu aroma de pere Frutti Fresh, 2.5 l
+Skipping duplicate product: Bautura carbogazoasa cu aroma de piersici Frutti Fresh, 2.5 l
+Skipping duplicate product: Bautura carbogazoasa cu aroma de struguri rosii Frutti Fresh, 2.5 l
+Skipping duplicate product: Bautura carbogazoasa cu aroma de struguri albi Frutti Fresh, 2.5 l</t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Bautura necarbogazoasa cu aloe vera Alloes, 1.5 l</t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Pulpe intregi cu spate Auchan, +/- 1 kg
+Skipping duplicate product: Piept de pui dezosat Auchan, fara piele, +/- 1 kg
+Skipping duplicate product: Aripi de pui sectionate Auchan, +/- 1 kg
+Skipping duplicate product: Ficat de pui Auchan, +/- 1 kg
+Skipping duplicate product: Pulpe inferioare de pui Auchan, +/- 1 kg
+Skipping duplicate product: Aripi de pui Auchan, +/- 1 kg
+Skipping duplicate product: Spinari cu aripi de pui Auchan, +/- 1 kg
+Skipping duplicate product: Pulpe inferioare de pui Auchan, +/- 1 kg
+Skipping duplicate product: Pui grill Auchan, +/- 1.5 kg
+Skipping duplicate product: Pulpe intregi cu spate Auchan, +/- 1 kg
+Skipping duplicate product: Aripi de pui sectionate Auchan, +/- 1 kg
+Skipping duplicate product: Ficat de pui Auchan, +/- 1 kg
+Skipping duplicate product: Pipote si inimi de pui Auchan, +/- 1 kg
+Skipping duplicate product: Aripi de pui Auchan, +/- 1 kg
+Skipping duplicate product: Inner de pui Auchan, +/- 1 kg
+Skipping duplicate product: Spinari cu aripi de pui Auchan, +/- 1 kg
+Skipping duplicate product: Piept de rata cu piele, +/- 1 kg
+Skipped 1 records due to missing required fields or errors
+Skipped 17 records due to duplicate product names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'</t>
+  </si>
+  <si>
+    <t>Skipping duplicate product: Ciocolata neagra Lindt Excellence, 100 g
+Skipping duplicate product: Ciocolata cu lapte Valor, fara gluten, 100 g
+Skipping duplicate product: Ciocolata cu caramel Milka, 100 g
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Ciocolata Rom Autentic Ghiceste Aroma, 80 g</t>
+  </si>
+  <si>
+    <t>Skipping duplicate product: Lapte de consum integral Monor, 3.5% grasime, 1 l
+Skipping duplicate product: Lapte de consum semidegresat Bonas, 1.8% grasime, 1 l</t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Muschi file Matache Macelaru, 100 g</t>
+  </si>
+  <si>
+    <t>Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Salam de vara Auchan, 500 g
+Error processing row: 'float' object has no attribute 'lower'
+Skipped 2 records due to missing required fields or errors
+Skipped 1 records due to duplicate product names</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ro/lactate-carne-mezeluri---peste/lactate/iaurt/c</t>
+  </si>
+  <si>
+    <t>Yohurt</t>
+  </si>
+  <si>
+    <t>Iaurt</t>
+  </si>
+  <si>
+    <t>lactate/iaurt</t>
+  </si>
+  <si>
+    <t>Category Auchan ID</t>
+  </si>
+  <si>
+    <t>https://www.auchan.ro/bacanie/ceai-si-cafea/cafea-macinata/c</t>
+  </si>
+  <si>
+    <t>Skipping duplicate product: Iaurt grecesc Olympus, 10% grasime, 150 g
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Iaurt de baut cu fibre Activia, 3 x 320 g
+Error processing row: 'float' object has no attribute 'lower'
+Skipping duplicate product: Iaurt de baut Actimel, cu afine si mure, 4 x 100 g
+Skipped 7 records due to missing required fields or errors
+Skipped 3 records due to duplicate product names</t>
   </si>
 </sst>
 </file>
@@ -319,13 +452,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,410 +775,747 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794095FE-BD26-6E45-A504-5D54BC82BC90}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G24" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.1640625" customWidth="1"/>
     <col min="2" max="3" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="98.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="75.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>77</v>
+      <c r="G1" t="s">
+        <v>78</v>
       </c>
       <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2">
+        <v>134</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2">
+        <v>134</v>
+      </c>
+      <c r="K2">
+        <f>SUM(F2:F249)</f>
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>366</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3">
+        <v>361</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F4">
+        <v>298</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4">
+        <v>294</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4">
+        <f>SUM(I2:I68)</f>
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5">
+        <v>508</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5">
+        <v>489</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>135</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <f>SUM(E2:E249)</f>
-        <v>3644</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3">
-        <v>366</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4">
-        <v>298</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>508</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1"/>
+      <c r="F6">
         <v>191</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6">
+        <v>173</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7">
         <v>68</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7">
+        <v>67</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8">
+        <v>199</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>3060100</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9">
+        <v>86</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>120</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10">
+        <v>120</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>272</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11">
+        <v>272</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12">
+        <v>41</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12">
+        <v>40</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>109</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13">
+        <v>108</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>247</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14">
+        <v>246</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>200</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>122</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11">
-        <v>277</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12">
-        <v>41</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13">
-        <v>109</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14">
-        <v>247</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15">
+      <c r="F15">
         <v>415</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15">
+        <v>410</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>133</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16">
+        <v>133</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>103</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17">
+        <v>101</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18">
+        <v>247</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18">
+        <v>244</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18">
-        <v>247</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19">
+      <c r="F19">
         <v>184</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19">
+        <v>181</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20">
+        <v>2030300</v>
+      </c>
+      <c r="F20">
+        <v>467</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20">
+        <v>440</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K21" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K22" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K24" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K25" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K26" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K27" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K28" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K29" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K31" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K32" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K33" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K34" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K35" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K36" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
     <sortCondition ref="A1:A20"/>
   </sortState>
   <hyperlinks>
@@ -1053,6 +1524,9 @@
     <hyperlink ref="D18" r:id="rId3" xr:uid="{6A98317F-2A8E-EA4D-8572-AE4CFD10035C}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{EE343B39-8D2C-944F-913F-15D9F7DECBFC}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{D6CF36FD-F048-9B4B-B02D-96A297E336C3}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{B494ACE2-B971-AA4E-801C-436EAFA8877A}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{46FE4B43-C46D-364D-BD58-811B9A3846D2}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{277F11D4-53D5-554C-B0C3-5628B463A91A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
[PURIO] Fixes for processor
</commit_message>
<xml_diff>
--- a/category_check_list.xlsx
+++ b/category_check_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmakonst/Documents/Projects/food_facts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7709C-7226-E142-B272-CB8F85D079DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A677BBDA-88FE-974E-8693-D7A9D8337F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44080" yWindow="-16660" windowWidth="30220" windowHeight="17940" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
+    <workbookView xWindow="-33900" yWindow="-16360" windowWidth="30220" windowHeight="17940" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,14 +452,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -778,7 +777,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G25"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,7 +790,7 @@
     <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -822,7 +821,7 @@
       <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" t="s">
         <v>80</v>
       </c>
       <c r="K1" t="s">
@@ -886,7 +885,7 @@
       <c r="I3">
         <v>361</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" t="s">
         <v>84</v>
       </c>
       <c r="K3" t="s">
@@ -918,7 +917,7 @@
       <c r="I4">
         <v>294</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" t="s">
         <v>85</v>
       </c>
       <c r="K4">
@@ -951,10 +950,10 @@
       <c r="I5">
         <v>489</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -984,10 +983,10 @@
       <c r="I6">
         <v>173</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1017,10 +1016,10 @@
       <c r="I7">
         <v>67</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1049,10 +1048,10 @@
       <c r="I8">
         <v>199</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1084,7 +1083,7 @@
       <c r="I9">
         <v>86</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1113,7 +1112,7 @@
       <c r="I10">
         <v>120</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1142,7 +1141,7 @@
       <c r="I11">
         <v>272</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1171,10 +1170,10 @@
       <c r="I12">
         <v>40</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" t="s">
         <v>88</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1203,10 +1202,10 @@
       <c r="I13">
         <v>108</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" t="s">
         <v>88</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1235,10 +1234,10 @@
       <c r="I14">
         <v>246</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1267,10 +1266,10 @@
       <c r="I15">
         <v>410</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" t="s">
         <v>89</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1299,7 +1298,7 @@
       <c r="I16">
         <v>133</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1328,10 +1327,10 @@
       <c r="I17">
         <v>101</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1360,10 +1359,10 @@
       <c r="I18">
         <v>244</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1392,10 +1391,10 @@
       <c r="I19">
         <v>181</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1427,90 +1426,90 @@
       <c r="I20">
         <v>440</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" t="s">
         <v>99</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K21" s="4" t="s">
+      <c r="K21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K22" s="4" t="s">
+      <c r="K22" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K23" s="4" t="s">
+      <c r="K23" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K24" s="4" t="s">
+      <c r="K24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K25" s="4" t="s">
+      <c r="K25" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K26" s="4" t="s">
+      <c r="K26" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K27" s="4" t="s">
+      <c r="K27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K28" s="4" t="s">
+      <c r="K28" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K29" s="4" t="s">
+      <c r="K29" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K30" s="4" t="s">
+      <c r="K30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K31" s="4" t="s">
+      <c r="K31" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K32" s="4" t="s">
+      <c r="K32" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K33" s="4" t="s">
+      <c r="K33" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K34" s="4" t="s">
+      <c r="K34" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K35" s="4" t="s">
+      <c r="K35" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K36" s="4" t="s">
+      <c r="K36" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add processor for one product
</commit_message>
<xml_diff>
--- a/category_check_list.xlsx
+++ b/category_check_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmakonst/Documents/Projects/food_facts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7410B44-1367-844F-81DA-14D4C3BCF304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD631A2-EA5D-ED40-A075-6553F57817BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16960" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
+    <workbookView xWindow="-39100" yWindow="-16060" windowWidth="36360" windowHeight="22640" xr2:uid="{2A516B36-17A3-7F4C-BA3B-AE289D5EB771}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="401">
   <si>
     <t>Category name</t>
   </si>
@@ -922,9 +922,6 @@
     <t>https://www.auchan.ro/bauturi-si-tutun/apa/apa-aromatizata/c</t>
   </si>
   <si>
-    <t>Juice</t>
-  </si>
-  <si>
     <t>Sucuri naturale si Nectar</t>
   </si>
   <si>
@@ -1039,9 +1036,6 @@
     <t>https://www.auchan.ro/fructe-si-legume/fructe-si-legume-uscate/fructe-deshidratate-si-confiate/c</t>
   </si>
   <si>
-    <t>Inghetata la caserola</t>
-  </si>
-  <si>
     <t>Inghetata la cornet si vafa</t>
   </si>
   <si>
@@ -1141,9 +1135,6 @@
     <t>https://www.auchan.ro/brutarie-cofetarie-gastro/paine/paine-proaspata-auchan/c</t>
   </si>
   <si>
-    <t>Bread</t>
-  </si>
-  <si>
     <t>Chifle, Baghete si Lipii</t>
   </si>
   <si>
@@ -1243,10 +1234,10 @@
     <t>All others were already in DB</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t xml:space="preserve"> e322i was not used in calculation</t>
+  </si>
+  <si>
+    <t>Do we reall need it</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1355,6 +1346,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1670,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794095FE-BD26-6E45-A504-5D54BC82BC90}">
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E141" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1741,8 +1734,8 @@
         <v>136</v>
       </c>
       <c r="I2" s="5">
-        <f>SUM(E2:E239)</f>
-        <v>12396</v>
+        <f>SUM(E2:E235)</f>
+        <v>14655</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1789,8 +1782,8 @@
         <v>294</v>
       </c>
       <c r="I4">
-        <f>SUM(G2:G67)</f>
-        <v>9041</v>
+        <f>SUM(G2:G364)</f>
+        <v>13689</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1">
@@ -2996,7 +2989,7 @@
         <v>98</v>
       </c>
       <c r="H54" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3518,6 +3511,12 @@
       <c r="E77">
         <v>326</v>
       </c>
+      <c r="F77" t="s">
+        <v>58</v>
+      </c>
+      <c r="G77">
+        <v>324</v>
+      </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="4" t="s">
@@ -3536,7 +3535,10 @@
         <v>112</v>
       </c>
       <c r="F78" t="s">
-        <v>402</v>
+        <v>58</v>
+      </c>
+      <c r="G78">
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3585,10 +3587,10 @@
         <v>100</v>
       </c>
       <c r="H80" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="4" t="s">
         <v>241</v>
       </c>
@@ -3605,10 +3607,13 @@
         <v>117</v>
       </c>
       <c r="F81" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G81">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="4" t="s">
         <v>244</v>
       </c>
@@ -3631,7 +3636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:8">
       <c r="A83" s="4" t="s">
         <v>247</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:8">
       <c r="A84" s="4" t="s">
         <v>250</v>
       </c>
@@ -3677,7 +3682,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:8">
       <c r="A85" s="4" t="s">
         <v>253</v>
       </c>
@@ -3700,7 +3705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:8">
       <c r="A86" s="4" t="s">
         <v>256</v>
       </c>
@@ -3717,10 +3722,13 @@
         <v>108</v>
       </c>
       <c r="F86" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G86">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="4" t="s">
         <v>259</v>
       </c>
@@ -3743,7 +3751,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:8">
       <c r="A88" s="9" t="s">
         <v>262</v>
       </c>
@@ -3766,7 +3774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:8">
       <c r="A89" s="4" t="s">
         <v>265</v>
       </c>
@@ -3782,8 +3790,14 @@
       <c r="E89">
         <v>315</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="F89" t="s">
+        <v>58</v>
+      </c>
+      <c r="G89">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="9" t="s">
         <v>268</v>
       </c>
@@ -3799,8 +3813,14 @@
       <c r="E90">
         <v>104</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="F90" t="s">
+        <v>58</v>
+      </c>
+      <c r="G90">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="4" t="s">
         <v>271</v>
       </c>
@@ -3816,8 +3836,14 @@
       <c r="E91">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="F91" t="s">
+        <v>58</v>
+      </c>
+      <c r="G91">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="4" t="s">
         <v>274</v>
       </c>
@@ -3833,8 +3859,14 @@
       <c r="E92">
         <v>75</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="F92" t="s">
+        <v>58</v>
+      </c>
+      <c r="G92">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="4" t="s">
         <v>277</v>
       </c>
@@ -3850,25 +3882,34 @@
       <c r="E93">
         <v>38</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="4" t="s">
+      <c r="F93" t="s">
+        <v>58</v>
+      </c>
+      <c r="G93">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" s="5" customFormat="1">
+      <c r="A94" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D94" s="11">
         <v>3120000</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="5">
         <v>128</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="4" t="s">
         <v>283</v>
       </c>
@@ -3881,8 +3922,17 @@
       <c r="D95" s="7">
         <v>3090600</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="E95">
+        <v>55</v>
+      </c>
+      <c r="F95" t="s">
+        <v>58</v>
+      </c>
+      <c r="G95">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="4" t="s">
         <v>286</v>
       </c>
@@ -3895,8 +3945,17 @@
       <c r="D96" s="7">
         <v>3090800</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>31</v>
+      </c>
+      <c r="F96" t="s">
+        <v>58</v>
+      </c>
+      <c r="G96">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="4" t="s">
         <v>289</v>
       </c>
@@ -3909,8 +3968,17 @@
       <c r="D97" s="7">
         <v>3090400</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>35</v>
+      </c>
+      <c r="F97" t="s">
+        <v>58</v>
+      </c>
+      <c r="G97">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="4" t="s">
         <v>292</v>
       </c>
@@ -3923,567 +3991,811 @@
       <c r="D98" s="7">
         <v>5010100</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="4" t="s">
-        <v>36</v>
+      <c r="E98">
+        <v>35</v>
+      </c>
+      <c r="F98" t="s">
+        <v>58</v>
+      </c>
+      <c r="G98">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="9" t="s">
+        <v>295</v>
       </c>
       <c r="B99" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>34</v>
+        <v>297</v>
       </c>
       <c r="D99" s="7">
-        <v>5060100</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="4" t="s">
+        <v>5060800</v>
+      </c>
+      <c r="E99">
+        <v>292</v>
+      </c>
+      <c r="F99" t="s">
+        <v>58</v>
+      </c>
+      <c r="G99">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>298</v>
+      </c>
+      <c r="B100" t="s">
+        <v>299</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D100" s="7">
+        <v>5060300</v>
+      </c>
+      <c r="E100">
+        <v>52</v>
+      </c>
+      <c r="F100" t="s">
+        <v>58</v>
+      </c>
+      <c r="G100">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>301</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D101" s="7">
+        <v>5060500</v>
+      </c>
+      <c r="E101">
+        <v>58</v>
+      </c>
+      <c r="F101" t="s">
+        <v>58</v>
+      </c>
+      <c r="G101">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>303</v>
+      </c>
+      <c r="B102" t="s">
+        <v>304</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D102" s="7">
+        <v>5060600</v>
+      </c>
+      <c r="E102">
+        <v>50</v>
+      </c>
+      <c r="F102" t="s">
+        <v>58</v>
+      </c>
+      <c r="G102">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B103" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D103" s="7">
+        <v>5060400</v>
+      </c>
+      <c r="E103">
+        <v>97</v>
+      </c>
+      <c r="F103" t="s">
+        <v>58</v>
+      </c>
+      <c r="G103">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D104" s="7">
+        <v>5080500</v>
+      </c>
+      <c r="E104">
+        <v>10</v>
+      </c>
+      <c r="F104" t="s">
+        <v>58</v>
+      </c>
+      <c r="G104">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D105" s="7">
+        <v>5040100</v>
+      </c>
+      <c r="E105">
+        <v>82</v>
+      </c>
+      <c r="F105" t="s">
+        <v>58</v>
+      </c>
+      <c r="G105">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="s">
+        <v>316</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D106" s="7">
+        <v>5040200</v>
+      </c>
+      <c r="E106">
+        <v>74</v>
+      </c>
+      <c r="F106" t="s">
+        <v>58</v>
+      </c>
+      <c r="G106">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B107" t="s">
+        <v>319</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D107" s="7">
+        <v>5040300</v>
+      </c>
+      <c r="E107">
+        <v>50</v>
+      </c>
+      <c r="F107" t="s">
+        <v>58</v>
+      </c>
+      <c r="G107">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" s="5" customFormat="1">
+      <c r="A108" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D108" s="11">
+        <v>1050100</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="5" customFormat="1">
+      <c r="A109" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D109" s="11">
+        <v>1050200</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" t="s">
+        <v>328</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D110" s="7">
+        <v>1030300</v>
+      </c>
+      <c r="E110">
+        <v>54</v>
+      </c>
+      <c r="F110" t="s">
+        <v>58</v>
+      </c>
+      <c r="G110">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B111" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D111" s="7">
+        <v>1030100</v>
+      </c>
+      <c r="E111">
+        <v>103</v>
+      </c>
+      <c r="F111" t="s">
+        <v>58</v>
+      </c>
+      <c r="G111">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D112" s="7">
+        <v>13010100</v>
+      </c>
+      <c r="E112">
+        <v>101</v>
+      </c>
+      <c r="F112" t="s">
+        <v>58</v>
+      </c>
+      <c r="G112">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B113" t="s">
+        <v>69</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D113" s="7">
+        <v>13010300</v>
+      </c>
+      <c r="E113">
+        <v>215</v>
+      </c>
+      <c r="F113" t="s">
+        <v>58</v>
+      </c>
+      <c r="G113">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B114" t="s">
+        <v>338</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D114" s="7">
+        <v>13020100</v>
+      </c>
+      <c r="E114">
+        <v>182</v>
+      </c>
+      <c r="F114" t="s">
+        <v>58</v>
+      </c>
+      <c r="G114">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>340</v>
+      </c>
+      <c r="B115" t="s">
+        <v>341</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D115" s="7">
+        <v>13020200</v>
+      </c>
+      <c r="E115">
         <v>39</v>
       </c>
-      <c r="B100" t="s">
-        <v>295</v>
-      </c>
-      <c r="C100" s="1" t="s">
+      <c r="F115" t="s">
+        <v>58</v>
+      </c>
+      <c r="G115">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>343</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D116" s="7">
+        <v>13050100</v>
+      </c>
+      <c r="E116">
+        <v>60</v>
+      </c>
+      <c r="F116" t="s">
+        <v>58</v>
+      </c>
+      <c r="G116">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B117" t="s">
+        <v>346</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D117" s="7">
+        <v>13050200</v>
+      </c>
+      <c r="E117">
+        <v>106</v>
+      </c>
+      <c r="F117" t="s">
+        <v>58</v>
+      </c>
+      <c r="G117">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B118" t="s">
+        <v>349</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D118" s="7">
+        <v>13040100</v>
+      </c>
+      <c r="E118">
+        <v>52</v>
+      </c>
+      <c r="F118" t="s">
+        <v>58</v>
+      </c>
+      <c r="G118">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B119" t="s">
+        <v>352</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D119" s="7">
+        <v>13040200</v>
+      </c>
+      <c r="E119">
+        <v>74</v>
+      </c>
+      <c r="F119" t="s">
+        <v>58</v>
+      </c>
+      <c r="G119">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="5" customFormat="1">
+      <c r="A120" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D120" s="11">
+        <v>13030100</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" s="5" customFormat="1">
+      <c r="A121" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D121" s="11">
+        <v>13030200</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" s="5" customFormat="1">
+      <c r="A122" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D122" s="11">
+        <v>13030300</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" s="5" customFormat="1" ht="17" customHeight="1">
+      <c r="A123" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D123" s="11">
+        <v>4030300</v>
+      </c>
+      <c r="H123" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" s="5" customFormat="1">
+      <c r="A124" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D124" s="11">
+        <v>4030100</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B125" t="s">
+        <v>370</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D125" s="7">
+        <v>4030400</v>
+      </c>
+      <c r="E125">
+        <v>31</v>
+      </c>
+      <c r="F125" t="s">
+        <v>58</v>
+      </c>
+      <c r="G125">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D126" s="7">
+        <v>4020900</v>
+      </c>
+      <c r="E126">
+        <v>10</v>
+      </c>
+      <c r="F126" t="s">
+        <v>58</v>
+      </c>
+      <c r="G126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D127" s="7">
+        <v>4020300</v>
+      </c>
+      <c r="E127">
+        <v>13</v>
+      </c>
+      <c r="F127" t="s">
+        <v>58</v>
+      </c>
+      <c r="G127">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>377</v>
+      </c>
+      <c r="B128" t="s">
+        <v>377</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D128" s="7">
+        <v>4020600</v>
+      </c>
+      <c r="E128">
+        <v>67</v>
+      </c>
+      <c r="F128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G128">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B129" t="s">
+        <v>380</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D129" s="7">
+        <v>4020800</v>
+      </c>
+      <c r="E129">
+        <v>10</v>
+      </c>
+      <c r="F129" t="s">
+        <v>58</v>
+      </c>
+      <c r="G129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B130" t="s">
+        <v>383</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D130" s="7">
+        <v>4020700</v>
+      </c>
+      <c r="E130">
+        <v>30</v>
+      </c>
+      <c r="F130" t="s">
+        <v>58</v>
+      </c>
+      <c r="G130">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D131" s="7">
+        <v>4010100</v>
+      </c>
+      <c r="E131">
+        <v>58</v>
+      </c>
+      <c r="F131" t="s">
+        <v>58</v>
+      </c>
+      <c r="G131">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B132" t="s">
+        <v>388</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D132" s="7">
+        <v>4010300</v>
+      </c>
+      <c r="E132">
+        <v>39</v>
+      </c>
+      <c r="F132" t="s">
+        <v>58</v>
+      </c>
+      <c r="G132">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B133" t="s">
+        <v>391</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D133" s="7">
+        <v>4040500</v>
+      </c>
+      <c r="E133">
+        <v>45</v>
+      </c>
+      <c r="F133" t="s">
+        <v>58</v>
+      </c>
+      <c r="G133">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D134" s="7">
+        <v>4040200</v>
+      </c>
+      <c r="E134">
         <v>38</v>
       </c>
-      <c r="D100" s="7">
-        <v>5060200</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="B101" t="s">
-        <v>297</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D101" s="7">
-        <v>5060800</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" t="s">
-        <v>299</v>
-      </c>
-      <c r="B102" t="s">
-        <v>300</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D102" s="7">
-        <v>5060300</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" t="s">
-        <v>302</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D103" s="7">
-        <v>5060500</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" t="s">
-        <v>304</v>
-      </c>
-      <c r="B104" t="s">
-        <v>305</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D104" s="7">
-        <v>5060600</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B105" t="s">
-        <v>308</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D105" s="7">
-        <v>5060400</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B106" t="s">
-        <v>311</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D106" s="7">
-        <v>5080500</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B107" t="s">
-        <v>314</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D107" s="7">
-        <v>5040100</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B108" t="s">
-        <v>317</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D108" s="7">
-        <v>5040200</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="B109" t="s">
-        <v>320</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D109" s="7">
-        <v>5040300</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B110" t="s">
-        <v>323</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D110" s="7">
-        <v>1050100</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="B111" t="s">
-        <v>326</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D111" s="7">
-        <v>1050200</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="B112" t="s">
-        <v>329</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="D112" s="7">
-        <v>1030300</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B113" t="s">
-        <v>332</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D113" s="7">
-        <v>1030100</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="B114" t="s">
-        <v>69</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D114" s="7">
-        <v>13010200</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="B115" t="s">
-        <v>69</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D115" s="7">
-        <v>13010100</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="B116" t="s">
-        <v>69</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D116" s="7">
-        <v>13010300</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B117" t="s">
-        <v>340</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D117" s="7">
-        <v>13020100</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" t="s">
-        <v>342</v>
-      </c>
-      <c r="B118" t="s">
-        <v>343</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D118" s="7">
-        <v>13020200</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" t="s">
-        <v>345</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="D119" s="7">
-        <v>13050100</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="B120" t="s">
-        <v>348</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D120" s="7">
-        <v>13050200</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B121" t="s">
-        <v>351</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D121" s="7">
-        <v>13040100</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="B122" t="s">
-        <v>354</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D122" s="7">
-        <v>13040200</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="B123" t="s">
-        <v>357</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D123" s="7">
-        <v>13030100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" t="s">
-        <v>359</v>
-      </c>
-      <c r="B124" t="s">
-        <v>360</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D124" s="7">
-        <v>13030200</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
-        <v>362</v>
-      </c>
-      <c r="B125" t="s">
-        <v>363</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D125" s="7">
-        <v>13030300</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
-        <v>365</v>
-      </c>
-      <c r="B126" t="s">
-        <v>366</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D126" s="7">
-        <v>4030300</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" t="s">
-        <v>74</v>
-      </c>
-      <c r="B127" t="s">
-        <v>368</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D127" s="7">
-        <v>4030200</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="A128" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B128" t="s">
-        <v>370</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D128" s="7">
-        <v>4030100</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="B129" t="s">
-        <v>373</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D129" s="7">
-        <v>4030400</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D130" s="7">
-        <v>4020900</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" t="s">
-        <v>377</v>
-      </c>
-      <c r="B131" t="s">
-        <v>378</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D131" s="7">
-        <v>4020300</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132" t="s">
-        <v>380</v>
-      </c>
-      <c r="B132" t="s">
-        <v>380</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D132" s="7">
-        <v>4020600</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="B133" t="s">
-        <v>383</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D133" s="7">
-        <v>4020800</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="B134" t="s">
-        <v>386</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="D134" s="7">
-        <v>4020700</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="F134" t="s">
+        <v>58</v>
+      </c>
+      <c r="G134">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" s="4" t="s">
-        <v>388</v>
+        <v>395</v>
+      </c>
+      <c r="B135" t="s">
+        <v>396</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="D135" s="7">
-        <v>4010100</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B136" t="s">
-        <v>391</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="D136" s="7">
-        <v>4010300</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="B137" t="s">
-        <v>394</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D137" s="7">
-        <v>4040500</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D138" s="7">
-        <v>4040200</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="B139" t="s">
-        <v>399</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D139" s="7">
         <v>4040100</v>
+      </c>
+      <c r="E135">
+        <v>11</v>
+      </c>
+      <c r="F135" t="s">
+        <v>58</v>
+      </c>
+      <c r="G135">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -4571,48 +4883,44 @@
     <hyperlink ref="C96" r:id="rId81" xr:uid="{260868B4-1BE7-DB42-BE68-0FBE038BE454}"/>
     <hyperlink ref="C97" r:id="rId82" xr:uid="{4D5C8DE0-1A36-C541-A8FF-F791B57C1821}"/>
     <hyperlink ref="C98" r:id="rId83" xr:uid="{06C98B24-DB02-B443-918B-2D37EB04F851}"/>
-    <hyperlink ref="C99" r:id="rId84" xr:uid="{AE81CA88-C3A8-5848-B6AD-E06F537C2825}"/>
-    <hyperlink ref="C100" r:id="rId85" xr:uid="{E609DA70-5220-7349-9E33-268C884C1AE7}"/>
-    <hyperlink ref="C101" r:id="rId86" xr:uid="{D5FA9C3F-C9CB-C942-A683-205B7EF213F2}"/>
-    <hyperlink ref="C102" r:id="rId87" xr:uid="{C91CFFCE-87F7-C646-BEE7-F2C691FB67F3}"/>
-    <hyperlink ref="C103" r:id="rId88" xr:uid="{C2950182-3EBD-264C-BDA6-0D15274317DA}"/>
-    <hyperlink ref="C104" r:id="rId89" xr:uid="{9E2B287C-7220-AA45-9035-3FB14A8AAC0B}"/>
-    <hyperlink ref="C105" r:id="rId90" xr:uid="{8C60DEB8-198A-1048-BEA1-DC08E6018A88}"/>
-    <hyperlink ref="C106" r:id="rId91" xr:uid="{7F175BDF-3C11-9546-8372-170EBBE3B834}"/>
-    <hyperlink ref="C107" r:id="rId92" xr:uid="{A9920CE8-E189-4F46-A060-1C99125AFF90}"/>
-    <hyperlink ref="C108" r:id="rId93" xr:uid="{88025615-284C-4040-904B-9944EC36A961}"/>
-    <hyperlink ref="C109" r:id="rId94" xr:uid="{89B709B6-3F2F-9746-BDA3-1ABE24AAE53C}"/>
-    <hyperlink ref="C110" r:id="rId95" xr:uid="{928BB6F7-27F1-7D48-B01E-EE38CB56D06C}"/>
-    <hyperlink ref="C111" r:id="rId96" xr:uid="{D334C47D-D7FD-9C44-B383-DAD017609FBC}"/>
-    <hyperlink ref="C112" r:id="rId97" xr:uid="{DF62F208-DED5-0C4A-9F62-2356F8569B51}"/>
-    <hyperlink ref="C113" r:id="rId98" xr:uid="{8C766735-0CD1-4644-8FC1-862660F29FCD}"/>
-    <hyperlink ref="C114" r:id="rId99" xr:uid="{52E47D22-5652-D14B-A3D1-23603C76F269}"/>
-    <hyperlink ref="C115" r:id="rId100" xr:uid="{E589B906-BA8E-B847-878A-1245523A9565}"/>
-    <hyperlink ref="C116" r:id="rId101" xr:uid="{E7991412-3ED1-C34C-8B2B-C4A90404A037}"/>
-    <hyperlink ref="C117" r:id="rId102" xr:uid="{EAD5C317-2CCA-C241-9A84-0D87B09DE592}"/>
-    <hyperlink ref="C118" r:id="rId103" xr:uid="{957FC88D-646C-E547-91BB-214659D3164A}"/>
-    <hyperlink ref="C119" r:id="rId104" xr:uid="{1EACD971-8C64-6844-9331-2F89CA59094F}"/>
-    <hyperlink ref="C120" r:id="rId105" xr:uid="{19A12EE2-43CE-5442-AD64-CA2418A1EA20}"/>
-    <hyperlink ref="C121" r:id="rId106" xr:uid="{9D4CFD82-1F19-AD47-8FE9-2991FE3AF9F5}"/>
-    <hyperlink ref="C122" r:id="rId107" xr:uid="{2D0AEC2C-A174-2B48-937C-3FE4697483E0}"/>
-    <hyperlink ref="C123" r:id="rId108" xr:uid="{34C85A2D-5DA1-2543-A350-93B0FF943477}"/>
-    <hyperlink ref="C124" r:id="rId109" xr:uid="{ABACCBF7-2833-F344-AD9D-5BE5132BA0D0}"/>
-    <hyperlink ref="C125" r:id="rId110" xr:uid="{CEFF3EB7-DC2F-C04E-9766-5C85FB027FA8}"/>
-    <hyperlink ref="C126" r:id="rId111" xr:uid="{D9085060-F9C1-4545-B45D-AE47DAA0B8CD}"/>
-    <hyperlink ref="C127" r:id="rId112" xr:uid="{ABAC541F-1081-BA4C-98FF-8FE4EF4D13CE}"/>
-    <hyperlink ref="C128" r:id="rId113" xr:uid="{6509F381-A5A1-B349-8E65-BA8C8938919A}"/>
-    <hyperlink ref="C129" r:id="rId114" xr:uid="{253B518A-1C29-5B4C-8332-A89420FAC88F}"/>
-    <hyperlink ref="C130" r:id="rId115" xr:uid="{1AB8979C-740D-F84A-AB05-18F4A7D992F9}"/>
-    <hyperlink ref="C131" r:id="rId116" xr:uid="{AEAF2D78-CA56-6F48-B414-79B6BE356EC6}"/>
-    <hyperlink ref="C132" r:id="rId117" xr:uid="{D4C4FD9A-AA65-5B41-9D2D-FA41C59FD325}"/>
-    <hyperlink ref="C133" r:id="rId118" xr:uid="{9CD5957E-A6B5-8D46-855F-D91F3297F8CC}"/>
-    <hyperlink ref="C134" r:id="rId119" xr:uid="{567FA327-4B26-5B49-89F8-6CB474CF43F4}"/>
-    <hyperlink ref="C135" r:id="rId120" xr:uid="{9F9535F2-2EC1-3241-A23A-E75136BB494A}"/>
-    <hyperlink ref="C136" r:id="rId121" xr:uid="{5D96E92F-66C8-2143-BF34-A0076F7921EE}"/>
-    <hyperlink ref="C137" r:id="rId122" xr:uid="{42FCC697-3BCE-884B-A7D3-BF222BB6E3B2}"/>
-    <hyperlink ref="C138" r:id="rId123" xr:uid="{4BDA0D71-3E4E-514C-BE78-1C1BD81FCECB}"/>
-    <hyperlink ref="C139" r:id="rId124" xr:uid="{551B79D6-008D-464C-BC53-DB1E4CEBAF60}"/>
-    <hyperlink ref="C26" r:id="rId125" xr:uid="{EB548499-D716-A74E-A755-37E0D4E8CE1E}"/>
+    <hyperlink ref="C99" r:id="rId84" xr:uid="{D5FA9C3F-C9CB-C942-A683-205B7EF213F2}"/>
+    <hyperlink ref="C100" r:id="rId85" xr:uid="{C91CFFCE-87F7-C646-BEE7-F2C691FB67F3}"/>
+    <hyperlink ref="C101" r:id="rId86" xr:uid="{C2950182-3EBD-264C-BDA6-0D15274317DA}"/>
+    <hyperlink ref="C102" r:id="rId87" xr:uid="{9E2B287C-7220-AA45-9035-3FB14A8AAC0B}"/>
+    <hyperlink ref="C103" r:id="rId88" xr:uid="{8C60DEB8-198A-1048-BEA1-DC08E6018A88}"/>
+    <hyperlink ref="C104" r:id="rId89" xr:uid="{7F175BDF-3C11-9546-8372-170EBBE3B834}"/>
+    <hyperlink ref="C105" r:id="rId90" xr:uid="{A9920CE8-E189-4F46-A060-1C99125AFF90}"/>
+    <hyperlink ref="C106" r:id="rId91" xr:uid="{88025615-284C-4040-904B-9944EC36A961}"/>
+    <hyperlink ref="C107" r:id="rId92" xr:uid="{89B709B6-3F2F-9746-BDA3-1ABE24AAE53C}"/>
+    <hyperlink ref="C108" r:id="rId93" xr:uid="{928BB6F7-27F1-7D48-B01E-EE38CB56D06C}"/>
+    <hyperlink ref="C109" r:id="rId94" xr:uid="{D334C47D-D7FD-9C44-B383-DAD017609FBC}"/>
+    <hyperlink ref="C110" r:id="rId95" xr:uid="{DF62F208-DED5-0C4A-9F62-2356F8569B51}"/>
+    <hyperlink ref="C111" r:id="rId96" xr:uid="{8C766735-0CD1-4644-8FC1-862660F29FCD}"/>
+    <hyperlink ref="C112" r:id="rId97" xr:uid="{E589B906-BA8E-B847-878A-1245523A9565}"/>
+    <hyperlink ref="C113" r:id="rId98" xr:uid="{E7991412-3ED1-C34C-8B2B-C4A90404A037}"/>
+    <hyperlink ref="C114" r:id="rId99" xr:uid="{EAD5C317-2CCA-C241-9A84-0D87B09DE592}"/>
+    <hyperlink ref="C115" r:id="rId100" xr:uid="{957FC88D-646C-E547-91BB-214659D3164A}"/>
+    <hyperlink ref="C116" r:id="rId101" xr:uid="{1EACD971-8C64-6844-9331-2F89CA59094F}"/>
+    <hyperlink ref="C117" r:id="rId102" xr:uid="{19A12EE2-43CE-5442-AD64-CA2418A1EA20}"/>
+    <hyperlink ref="C118" r:id="rId103" xr:uid="{9D4CFD82-1F19-AD47-8FE9-2991FE3AF9F5}"/>
+    <hyperlink ref="C119" r:id="rId104" xr:uid="{2D0AEC2C-A174-2B48-937C-3FE4697483E0}"/>
+    <hyperlink ref="C120" r:id="rId105" xr:uid="{34C85A2D-5DA1-2543-A350-93B0FF943477}"/>
+    <hyperlink ref="C121" r:id="rId106" xr:uid="{ABACCBF7-2833-F344-AD9D-5BE5132BA0D0}"/>
+    <hyperlink ref="C122" r:id="rId107" xr:uid="{CEFF3EB7-DC2F-C04E-9766-5C85FB027FA8}"/>
+    <hyperlink ref="C123" r:id="rId108" xr:uid="{D9085060-F9C1-4545-B45D-AE47DAA0B8CD}"/>
+    <hyperlink ref="C124" r:id="rId109" xr:uid="{6509F381-A5A1-B349-8E65-BA8C8938919A}"/>
+    <hyperlink ref="C125" r:id="rId110" xr:uid="{253B518A-1C29-5B4C-8332-A89420FAC88F}"/>
+    <hyperlink ref="C126" r:id="rId111" xr:uid="{1AB8979C-740D-F84A-AB05-18F4A7D992F9}"/>
+    <hyperlink ref="C127" r:id="rId112" xr:uid="{AEAF2D78-CA56-6F48-B414-79B6BE356EC6}"/>
+    <hyperlink ref="C128" r:id="rId113" xr:uid="{D4C4FD9A-AA65-5B41-9D2D-FA41C59FD325}"/>
+    <hyperlink ref="C129" r:id="rId114" xr:uid="{9CD5957E-A6B5-8D46-855F-D91F3297F8CC}"/>
+    <hyperlink ref="C130" r:id="rId115" xr:uid="{567FA327-4B26-5B49-89F8-6CB474CF43F4}"/>
+    <hyperlink ref="C131" r:id="rId116" xr:uid="{9F9535F2-2EC1-3241-A23A-E75136BB494A}"/>
+    <hyperlink ref="C132" r:id="rId117" xr:uid="{5D96E92F-66C8-2143-BF34-A0076F7921EE}"/>
+    <hyperlink ref="C133" r:id="rId118" xr:uid="{42FCC697-3BCE-884B-A7D3-BF222BB6E3B2}"/>
+    <hyperlink ref="C134" r:id="rId119" xr:uid="{4BDA0D71-3E4E-514C-BE78-1C1BD81FCECB}"/>
+    <hyperlink ref="C135" r:id="rId120" xr:uid="{551B79D6-008D-464C-BC53-DB1E4CEBAF60}"/>
+    <hyperlink ref="C26" r:id="rId121" xr:uid="{EB548499-D716-A74E-A755-37E0D4E8CE1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>